<commit_message>
Updated Protocol Model following meeting
</commit_message>
<xml_diff>
--- a/Use Case Model/use case.xlsx
+++ b/Use Case Model/use case.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanis\Desktop\Git\MedievalWarfare\Use Case Model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="15315" windowHeight="7965"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>Play Medieval Warfare</t>
   </si>
@@ -214,13 +219,37 @@
   </si>
   <si>
     <t xml:space="preserve">Scope : </t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Server, UI</t>
+  </si>
+  <si>
+    <t>Server, UI, Player</t>
+  </si>
+  <si>
+    <t>Server, Player</t>
+  </si>
+  <si>
+    <t>Engine, Player,Server</t>
+  </si>
+  <si>
+    <t>Engine, UI</t>
+  </si>
+  <si>
+    <t>Engine, Map</t>
+  </si>
+  <si>
+    <t>Engine, UI, Map, Unit,Town</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,18 +266,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -403,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -417,9 +440,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -453,17 +473,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,7 +535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,9 +567,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -571,6 +602,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -746,14 +778,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="3" customWidth="1"/>
@@ -765,7 +797,7 @@
     <col min="8" max="8" width="14.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -785,21 +817,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -819,7 +857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="180">
+    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -839,7 +877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -859,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -879,69 +917,69 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>59</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" ht="30">
-      <c r="A10" s="8"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="1:8" ht="90">
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -957,7 +995,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -977,21 +1015,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="H25" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1011,7 +1055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="165">
+    <row r="27" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1031,7 +1075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -1051,7 +1095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -1071,53 +1115,53 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="5" t="s">
         <v>59</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="8"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30">
-      <c r="A32" s="8"/>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
       <c r="B32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="1:8" ht="105">
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1137,7 +1181,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
@@ -1151,17 +1195,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="5"/>
+      <c r="B52" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="D52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="E52" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="16"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
@@ -1175,7 +1224,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="135">
+    <row r="54" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
@@ -1189,7 +1238,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1203,7 +1252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -1217,39 +1266,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="45">
-      <c r="A58" s="8"/>
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
       <c r="B58" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D58" s="7"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30">
-      <c r="A59" s="9"/>
-      <c r="B59" s="10"/>
-      <c r="D59" s="8"/>
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="D59" s="7"/>
       <c r="E59" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14.25" customHeight="1">
+    <row r="60" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -1261,19 +1310,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:H11"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="D57:D59"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:E11"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:H11"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A57:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1281,26 +1330,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>